<commit_message>
FIX: Se corrigen botones caso error || éxito
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvida\Desktop\Temporal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\QR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC9C3D2-FF83-4573-8368-E9CADDF35BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C740CBB8-6E98-467F-895C-8AFC2E322ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="1680" windowWidth="23250" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Todos los Puntos de Medicion" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Código</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Ruta</t>
+  </si>
+  <si>
+    <t>Orden</t>
   </si>
 </sst>
 </file>
@@ -87,7 +90,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -101,11 +108,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B12" totalsRowShown="0">
-  <autoFilter ref="A1:B12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C12" totalsRowShown="0">
+  <autoFilter ref="A1:C12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="3">
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Código"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ruta"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Orden"/>
+    <tableColumn id="1" xr3:uid="{3DF5E59B-757B-43D7-90BB-4EEF04FB8D25}" name="Ruta" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -409,25 +417,62 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="dataSheet"/>
-  <dimension ref="A1:B147"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" s="4"/>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="2"/>
@@ -771,7 +816,7 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Longitud excedida" error="Este valor debe tener 100 caracteres o menos." promptTitle="Texto (se requiere)" prompt="Longitud máxima: 100 caracteres." sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>100</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Búsqueda (se requiere)" prompt="Este registro de Definición de recorrido ya tiene que existir en Microsoft Dynamics 365 o en este archivo de origen." sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Búsqueda (se requiere)" prompt="Este registro de Definición de recorrido ya tiene que existir en Microsoft Dynamics 365 o en este archivo de origen." sqref="B2:B1048576 C2:C12" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
FIX: Se modifica template
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\QR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C740CBB8-6E98-467F-895C-8AFC2E322ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59D83FE-9F95-4E12-BB66-CC29596BB3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Todos los Puntos de Medicion" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Código</t>
   </si>
@@ -44,17 +44,23 @@
     <t>Inactivo</t>
   </si>
   <si>
-    <t>Ruta</t>
-  </si>
-  <si>
     <t>Orden</t>
+  </si>
+  <si>
+    <t>Definición de recorrido</t>
+  </si>
+  <si>
+    <t>Equipo</t>
+  </si>
+  <si>
+    <t>Descripción</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -108,12 +114,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C12" totalsRowShown="0">
-  <autoFilter ref="A1:C12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0">
+  <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Código"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Orden"/>
-    <tableColumn id="1" xr3:uid="{3DF5E59B-757B-43D7-90BB-4EEF04FB8D25}" name="Ruta" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3DF5E59B-757B-43D7-90BB-4EEF04FB8D25}" name="Definición de recorrido" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{4C435318-3D16-4BD9-AD79-FCD085B6282F}" name="Equipo"/>
+    <tableColumn id="3" xr3:uid="{D2763DE0-282B-46EA-A85A-EB61680AB514}" name="Descripción"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -417,397 +425,403 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="dataSheet"/>
-  <dimension ref="A1:C147"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="4"/>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="4"/>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="4"/>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="4"/>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="4"/>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="4"/>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="4"/>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="4"/>
     </row>
@@ -832,14 +846,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -850,7 +864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>

</xml_diff>